<commit_message>
Fix a bunch of honorific mistakes and make other very minor tweaks (Primarily Nov-Dec Yayoi)
</commit_message>
<xml_diff>
--- a/stripped/P00110.mes.bin.xlsx
+++ b/stripped/P00110.mes.bin.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACFE78D-42E9-4957-8C53-398F4ACE916B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C178878-3C9C-4727-A8BC-330166E0B052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33810" yWindow="0" windowWidth="33900" windowHeight="21090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="5460" windowWidth="50850" windowHeight="21795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P00110.mes.bin" sheetId="1" r:id="rId1"/>

</xml_diff>